<commit_message>
Calibrate SoCEUtiNTY and SoCDTtiNTY
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
+++ b/InputData/bldgs/SoCEUtiNTY/Share of Cpnt E Use that is New This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\eps-eu\InputData\bldgs\SoCEUtiNTY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\bldgs\SoCEUtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99013A5-651A-4B13-AF61-3A587EAB588B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620164C6-1F09-4B7B-9688-7C748152420E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13815" yWindow="-12975" windowWidth="18945" windowHeight="11745" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1770,19 +1770,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1790,167 +1790,167 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="30" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B17" s="30" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B19" s="32">
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B24" s="30" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B25" s="33" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>379</v>
       </c>
@@ -1967,13 +1967,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.3984375" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="1" max="1" width="25.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>15.833333333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>51.81818181818182</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>9.1324200913242013</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>13.533333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2045,14 +2045,14 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="43.59765625" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="8.73046875" style="6"/>
+    <col min="1" max="1" width="19.81640625" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6328125" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
         <v>181</v>
       </c>
@@ -2165,8 +2165,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="23" t="s">
         <v>180</v>
       </c>
@@ -2177,7 +2177,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="23" t="s">
         <v>178</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="23" t="s">
         <v>175</v>
       </c>
@@ -2201,7 +2201,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="23" t="s">
         <v>173</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>339</v>
       </c>
@@ -2220,12 +2220,12 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="21" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
         <v>168</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="19" t="s">
         <v>166</v>
       </c>
@@ -2457,18 +2457,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>336</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>8.4399999999999996E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>334</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>1.0499E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>332</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>-7.2430000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>330</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>8.3569999999999998E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>329</v>
       </c>
@@ -3063,17 +3063,17 @@
         <v>3.7309999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>325</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>-7.7879999999999998E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>324</v>
       </c>
@@ -3311,12 +3311,12 @@
         <v>-8.8489999999999992E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>323</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>-1.1476E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>321</v>
       </c>
@@ -3554,17 +3554,17 @@
         <v>-1.2533000000000001E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>319</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>-1.041E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>318</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>6.9200000000000002E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>317</v>
       </c>
@@ -3921,7 +3921,7 @@
         <v>1.9040000000000001E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>316</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>3.362E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>315</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>1.0992999999999999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>314</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>8.9499999999999996E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>313</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>-2.4559999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>311</v>
       </c>
@@ -4516,7 +4516,7 @@
         <v>-1.7500999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>310</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>-9.953E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>308</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>1.2205000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>306</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>5.1910000000000003E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>304</v>
       </c>
@@ -4992,7 +4992,7 @@
         <v>-3.2238000000000003E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>302</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>-2.0820000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>300</v>
       </c>
@@ -5230,7 +5230,7 @@
         <v>6.9309999999999997E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>299</v>
       </c>
@@ -5349,12 +5349,12 @@
         <v>2.2339999999999999E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>298</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>2.9799999999999998E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>297</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>-7.4190000000000002E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>295</v>
       </c>
@@ -5711,7 +5711,7 @@
         <v>2.3839999999999998E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>294</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>3.7450000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="11" t="s">
         <v>293</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>6.659E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="11" t="s">
         <v>291</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>-5.071E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>289</v>
       </c>
@@ -6187,12 +6187,12 @@
         <v>8.1099999999999998E-4</v>
       </c>
     </row>
-    <row r="59" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
         <v>288</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>-1.4128E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
         <v>287</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>-3.7629999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>286</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>-6.2040000000000003E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
         <v>285</v>
       </c>
@@ -6668,12 +6668,12 @@
         <v>-1.5632E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="10" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
         <v>283</v>
       </c>
@@ -6792,7 +6792,7 @@
         <v>-7.0309999999999999E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="11" t="s">
         <v>281</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>-1.7628999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="11" t="s">
         <v>279</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>-5.5599999999999998E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
         <v>278</v>
       </c>
@@ -7149,7 +7149,7 @@
         <v>1.4448000000000001E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
         <v>277</v>
       </c>
@@ -7268,7 +7268,7 @@
         <v>-4.9649999999999998E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="11" t="s">
         <v>276</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>-6.3109999999999998E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="11" t="s">
         <v>274</v>
       </c>
@@ -7506,12 +7506,12 @@
         <v>-2.0202999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
         <v>272</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>-1.9480000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="11" t="s">
         <v>271</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>4.9600000000000002E-4</v>
       </c>
     </row>
-    <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="11" t="s">
         <v>270</v>
       </c>
@@ -7868,7 +7868,7 @@
         <v>1.214E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="11" t="s">
         <v>269</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>3.362E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="11" t="s">
         <v>268</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11" t="s">
         <v>267</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>8.5059999999999997E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11" t="s">
         <v>266</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>-2.4559999999999998E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="11" t="s">
         <v>265</v>
       </c>
@@ -8463,7 +8463,7 @@
         <v>-1.7500999999999999E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="11" t="s">
         <v>264</v>
       </c>
@@ -8582,7 +8582,7 @@
         <v>-9.953E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="11" t="s">
         <v>263</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>1.2205000000000001E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="11" t="s">
         <v>262</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>5.1910000000000003E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="11" t="s">
         <v>261</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>-3.2238000000000003E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="11" t="s">
         <v>260</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>-2.0820000000000001E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
         <v>259</v>
       </c>
@@ -9177,7 +9177,7 @@
         <v>5.6210000000000001E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="11" t="s">
         <v>258</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>5.04E-4</v>
       </c>
     </row>
-    <row r="92" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="11" t="s">
         <v>256</v>
       </c>
@@ -9415,12 +9415,12 @@
         <v>-1.823E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="11" t="s">
         <v>255</v>
       </c>
@@ -9539,7 +9539,7 @@
         <v>-2.343E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="11" t="s">
         <v>253</v>
       </c>
@@ -9658,7 +9658,7 @@
         <v>-1.9719999999999998E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="11" t="s">
         <v>251</v>
       </c>
@@ -9777,7 +9777,7 @@
         <v>1.2999999999999999E-4</v>
       </c>
     </row>
-    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="11" t="s">
         <v>249</v>
       </c>
@@ -9896,7 +9896,7 @@
         <v>7.3899999999999997E-4</v>
       </c>
     </row>
-    <row r="99" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="11" t="s">
         <v>247</v>
       </c>
@@ -10015,7 +10015,7 @@
         <v>6.1139999999999996E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="11" t="s">
         <v>245</v>
       </c>
@@ -10134,7 +10134,7 @@
         <v>6.339E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="11" t="s">
         <v>243</v>
       </c>
@@ -10253,7 +10253,7 @@
         <v>-5.0639999999999999E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="11" t="s">
         <v>241</v>
       </c>
@@ -10372,7 +10372,7 @@
         <v>-2.0070000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="11" t="s">
         <v>239</v>
       </c>
@@ -10491,7 +10491,7 @@
         <v>-1.2541999999999999E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="11" t="s">
         <v>237</v>
       </c>
@@ -10610,7 +10610,7 @@
         <v>9.5589999999999998E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="11" t="s">
         <v>235</v>
       </c>
@@ -10729,7 +10729,7 @@
         <v>2.562E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="11" t="s">
         <v>233</v>
       </c>
@@ -10848,7 +10848,7 @@
         <v>-3.4768E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="11" t="s">
         <v>231</v>
       </c>
@@ -10967,7 +10967,7 @@
         <v>-4.6909999999999999E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="11" t="s">
         <v>229</v>
       </c>
@@ -11086,7 +11086,7 @@
         <v>3.9480000000000001E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="11" t="s">
         <v>227</v>
       </c>
@@ -11205,12 +11205,12 @@
         <v>-5.6499999999999996E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="10" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="112" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="11" t="s">
         <v>224</v>
       </c>
@@ -11329,7 +11329,7 @@
         <v>2.7342999999999999E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="11" t="s">
         <v>222</v>
       </c>
@@ -11448,7 +11448,7 @@
         <v>2.7820999999999999E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="11" t="s">
         <v>220</v>
       </c>
@@ -11567,7 +11567,7 @@
         <v>9.7493999999999997E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="11" t="s">
         <v>219</v>
       </c>
@@ -11686,7 +11686,7 @@
         <v>9.724E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="11" t="s">
         <v>218</v>
       </c>
@@ -11805,12 +11805,12 @@
         <v>8.5554000000000005E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="11" t="s">
         <v>217</v>
       </c>
@@ -11929,7 +11929,7 @@
         <v>-1.8090000000000001E-3</v>
       </c>
     </row>
-    <row r="120" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="11" t="s">
         <v>216</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>-1.7240000000000001E-3</v>
       </c>
     </row>
-    <row r="121" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="11" t="s">
         <v>215</v>
       </c>
@@ -12167,7 +12167,7 @@
         <v>1.0460000000000001E-3</v>
       </c>
     </row>
-    <row r="122" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="11" t="s">
         <v>214</v>
       </c>
@@ -12286,7 +12286,7 @@
         <v>1.934E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="11" t="s">
         <v>213</v>
       </c>
@@ -12405,7 +12405,7 @@
         <v>-2.6310000000000001E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="11" t="s">
         <v>212</v>
       </c>
@@ -12524,7 +12524,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
     </row>
-    <row r="125" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="11" t="s">
         <v>211</v>
       </c>
@@ -12643,7 +12643,7 @@
         <v>1.5E-5</v>
       </c>
     </row>
-    <row r="126" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="11" t="s">
         <v>210</v>
       </c>
@@ -12762,7 +12762,7 @@
         <v>-9.4700000000000003E-4</v>
       </c>
     </row>
-    <row r="127" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="11" t="s">
         <v>209</v>
       </c>
@@ -12881,7 +12881,7 @@
         <v>1.7769999999999999E-3</v>
       </c>
     </row>
-    <row r="128" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="11" t="s">
         <v>208</v>
       </c>
@@ -13000,12 +13000,12 @@
         <v>-1.3990000000000001E-3</v>
       </c>
     </row>
-    <row r="130" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="131" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="11" t="s">
         <v>207</v>
       </c>
@@ -13124,7 +13124,7 @@
         <v>4.5779999999999996E-3</v>
       </c>
     </row>
-    <row r="132" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="11" t="s">
         <v>206</v>
       </c>
@@ -13243,7 +13243,7 @@
         <v>2.4529999999999999E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" s="11" t="s">
         <v>205</v>
       </c>
@@ -13362,7 +13362,7 @@
         <v>-3.9060000000000002E-3</v>
       </c>
     </row>
-    <row r="134" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" s="11" t="s">
         <v>204</v>
       </c>
@@ -13481,7 +13481,7 @@
         <v>-8.1899999999999996E-4</v>
       </c>
     </row>
-    <row r="135" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" s="11" t="s">
         <v>203</v>
       </c>
@@ -13600,7 +13600,7 @@
         <v>1.384E-3</v>
       </c>
     </row>
-    <row r="136" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="11" t="s">
         <v>202</v>
       </c>
@@ -13719,7 +13719,7 @@
         <v>-9.7400000000000004E-4</v>
       </c>
     </row>
-    <row r="137" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="11" t="s">
         <v>201</v>
       </c>
@@ -13838,7 +13838,7 @@
         <v>4.7860000000000003E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="11" t="s">
         <v>200</v>
       </c>
@@ -13957,7 +13957,7 @@
         <v>6.5649999999999997E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" s="11" t="s">
         <v>199</v>
       </c>
@@ -14076,7 +14076,7 @@
         <v>8.744E-3</v>
       </c>
     </row>
-    <row r="140" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="11" t="s">
         <v>198</v>
       </c>
@@ -14195,8 +14195,8 @@
         <v>4.3969999999999999E-3</v>
       </c>
     </row>
-    <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="142" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B142" s="35" t="s">
         <v>197</v>
       </c>
@@ -14238,102 +14238,102 @@
       <c r="AL142" s="35"/>
       <c r="AM142" s="35"/>
     </row>
-    <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B143" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="144" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B144" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B145" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B146" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B147" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B148" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B149" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="150" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B150" s="7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="151" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B151" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B152" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="153" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B153" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="154" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B154" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="155" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B155" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="156" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B156" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B157" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="158" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B158" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="159" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B159" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B160" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="161" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B161" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B162" s="7" t="s">
         <v>18</v>
       </c>
@@ -14358,14 +14358,14 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="43.59765625" style="6" customWidth="1"/>
-    <col min="3" max="16384" width="8.73046875" style="6"/>
+    <col min="1" max="1" width="19.81640625" style="6" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6328125" style="6" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="21" t="s">
         <v>181</v>
       </c>
@@ -14478,8 +14478,8 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="23" t="s">
         <v>180</v>
       </c>
@@ -14490,7 +14490,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
     </row>
-    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="23" t="s">
         <v>178</v>
       </c>
@@ -14503,7 +14503,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="23" t="s">
         <v>175</v>
       </c>
@@ -14514,7 +14514,7 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
     </row>
-    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="23" t="s">
         <v>173</v>
       </c>
@@ -14525,7 +14525,7 @@
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
     </row>
-    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>171</v>
       </c>
@@ -14533,12 +14533,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="21" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="21" t="s">
         <v>168</v>
       </c>
@@ -14654,7 +14654,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="19" t="s">
         <v>166</v>
       </c>
@@ -14770,18 +14770,18 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>163</v>
       </c>
@@ -14900,7 +14900,7 @@
         <v>1.0206E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>161</v>
       </c>
@@ -15019,7 +15019,7 @@
         <v>7.5760000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>159</v>
       </c>
@@ -15138,17 +15138,17 @@
         <v>1.0149999999999999E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>156</v>
       </c>
@@ -15267,7 +15267,7 @@
         <v>-5.5329999999999997E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>154</v>
       </c>
@@ -15386,7 +15386,7 @@
         <v>-8.9350000000000002E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>152</v>
       </c>
@@ -15505,17 +15505,17 @@
         <v>-7.2139999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>148</v>
       </c>
@@ -15634,7 +15634,7 @@
         <v>-3.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>147</v>
       </c>
@@ -15753,7 +15753,7 @@
         <v>-2.9450000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>146</v>
       </c>
@@ -15872,7 +15872,7 @@
         <v>-8.2909999999999998E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>145</v>
       </c>
@@ -15991,7 +15991,7 @@
         <v>-1.1093E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>144</v>
       </c>
@@ -16110,7 +16110,7 @@
         <v>-6.5640000000000004E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>143</v>
       </c>
@@ -16229,7 +16229,7 @@
         <v>-1.9772000000000001E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>142</v>
       </c>
@@ -16348,7 +16348,7 @@
         <v>-4.35E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>141</v>
       </c>
@@ -16467,7 +16467,7 @@
         <v>-1.0253E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>140</v>
       </c>
@@ -16586,7 +16586,7 @@
         <v>1.6978E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>139</v>
       </c>
@@ -16705,7 +16705,7 @@
         <v>1.7672E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>137</v>
       </c>
@@ -16824,12 +16824,12 @@
         <v>5.1929999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>135</v>
       </c>
@@ -16948,7 +16948,7 @@
         <v>-6.9439999999999997E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>134</v>
       </c>
@@ -17067,7 +17067,7 @@
         <v>-1.3974E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>133</v>
       </c>
@@ -17186,7 +17186,7 @@
         <v>1.438E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>132</v>
       </c>
@@ -17305,7 +17305,7 @@
         <v>9.7310000000000001E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>131</v>
       </c>
@@ -17424,7 +17424,7 @@
         <v>1.7788999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>129</v>
       </c>
@@ -17543,12 +17543,12 @@
         <v>4.705E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>127</v>
       </c>
@@ -17667,7 +17667,7 @@
         <v>-1.0187E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>126</v>
       </c>
@@ -17786,7 +17786,7 @@
         <v>2.7700000000000001E-4</v>
       </c>
     </row>
-    <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>125</v>
       </c>
@@ -17905,7 +17905,7 @@
         <v>2.6340000000000001E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>123</v>
       </c>
@@ -18024,7 +18024,7 @@
         <v>-4.4060000000000002E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="11" t="s">
         <v>122</v>
       </c>
@@ -18143,7 +18143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="11" t="s">
         <v>120</v>
       </c>
@@ -18262,12 +18262,12 @@
         <v>5.3270000000000001E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
         <v>117</v>
       </c>
@@ -18386,7 +18386,7 @@
         <v>-6.8739999999999999E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
         <v>116</v>
       </c>
@@ -18505,7 +18505,7 @@
         <v>-3.385E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
         <v>115</v>
       </c>
@@ -18624,7 +18624,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
         <v>114</v>
       </c>
@@ -18743,7 +18743,7 @@
         <v>-1.1093E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
         <v>113</v>
       </c>
@@ -18862,7 +18862,7 @@
         <v>7.0070000000000002E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
         <v>112</v>
       </c>
@@ -18981,7 +18981,7 @@
         <v>-1.9772000000000001E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="11" t="s">
         <v>111</v>
       </c>
@@ -19100,7 +19100,7 @@
         <v>-4.35E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="11" t="s">
         <v>110</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>-1.0253E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="11" t="s">
         <v>109</v>
       </c>
@@ -19338,7 +19338,7 @@
         <v>1.6978E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="11" t="s">
         <v>108</v>
       </c>
@@ -19457,7 +19457,7 @@
         <v>1.5339E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
         <v>107</v>
       </c>
@@ -19576,7 +19576,7 @@
         <v>4.561E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>105</v>
       </c>
@@ -19695,12 +19695,12 @@
         <v>1.1249999999999999E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="10" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
         <v>102</v>
       </c>
@@ -19819,7 +19819,7 @@
         <v>-6.5789999999999998E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="11" t="s">
         <v>100</v>
       </c>
@@ -19938,7 +19938,7 @@
         <v>-5.6740000000000002E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="11" t="s">
         <v>98</v>
       </c>
@@ -20057,7 +20057,7 @@
         <v>-3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="11" t="s">
         <v>96</v>
       </c>
@@ -20176,7 +20176,7 @@
         <v>-1.3679E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="11" t="s">
         <v>94</v>
       </c>
@@ -20295,7 +20295,7 @@
         <v>2.9090000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11" t="s">
         <v>92</v>
       </c>
@@ -20414,7 +20414,7 @@
         <v>-2.2335000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11" t="s">
         <v>90</v>
       </c>
@@ -20533,7 +20533,7 @@
         <v>-3.0479999999999999E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="11" t="s">
         <v>88</v>
       </c>
@@ -20652,7 +20652,7 @@
         <v>-1.2841E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="11" t="s">
         <v>86</v>
       </c>
@@ -20771,7 +20771,7 @@
         <v>1.4319E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="11" t="s">
         <v>84</v>
       </c>
@@ -20890,7 +20890,7 @@
         <v>1.4466E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="11" t="s">
         <v>82</v>
       </c>
@@ -21009,12 +21009,12 @@
         <v>2.8630000000000001E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
         <v>79</v>
       </c>
@@ -21133,7 +21133,7 @@
         <v>4.3639999999999998E-3</v>
       </c>
     </row>
-    <row r="90" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="11" t="s">
         <v>77</v>
       </c>
@@ -21252,7 +21252,7 @@
         <v>6.2715999999999994E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="11" t="s">
         <v>75</v>
       </c>
@@ -21371,7 +21371,7 @@
         <v>4.8741E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="11" t="s">
         <v>73</v>
       </c>
@@ -21490,12 +21490,12 @@
         <v>4.7280999999999997E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="11" t="s">
         <v>70</v>
       </c>
@@ -21614,7 +21614,7 @@
         <v>-1.8090000000000001E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="11" t="s">
         <v>69</v>
       </c>
@@ -21733,7 +21733,7 @@
         <v>-1.7240000000000001E-3</v>
       </c>
     </row>
-    <row r="97" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="11" t="s">
         <v>68</v>
       </c>
@@ -21852,7 +21852,7 @@
         <v>1.0460000000000001E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="11" t="s">
         <v>67</v>
       </c>
@@ -21971,7 +21971,7 @@
         <v>1.934E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="11" t="s">
         <v>66</v>
       </c>
@@ -22090,7 +22090,7 @@
         <v>-2.6310000000000001E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="11" t="s">
         <v>65</v>
       </c>
@@ -22209,7 +22209,7 @@
         <v>4.5800000000000002E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="11" t="s">
         <v>64</v>
       </c>
@@ -22328,7 +22328,7 @@
         <v>1.5E-5</v>
       </c>
     </row>
-    <row r="102" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="11" t="s">
         <v>63</v>
       </c>
@@ -22447,7 +22447,7 @@
         <v>-9.4700000000000003E-4</v>
       </c>
     </row>
-    <row r="103" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="11" t="s">
         <v>62</v>
       </c>
@@ -22566,7 +22566,7 @@
         <v>1.7769999999999999E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="11" t="s">
         <v>61</v>
       </c>
@@ -22685,12 +22685,12 @@
         <v>-1.3990000000000001E-3</v>
       </c>
     </row>
-    <row r="106" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="11" t="s">
         <v>59</v>
       </c>
@@ -22809,7 +22809,7 @@
         <v>4.5779999999999996E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="11" t="s">
         <v>57</v>
       </c>
@@ -22928,7 +22928,7 @@
         <v>2.4529999999999999E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="11" t="s">
         <v>55</v>
       </c>
@@ -23047,7 +23047,7 @@
         <v>-3.9060000000000002E-3</v>
       </c>
     </row>
-    <row r="110" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="11" t="s">
         <v>53</v>
       </c>
@@ -23166,7 +23166,7 @@
         <v>-8.1899999999999996E-4</v>
       </c>
     </row>
-    <row r="111" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="11" t="s">
         <v>51</v>
       </c>
@@ -23285,7 +23285,7 @@
         <v>1.384E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="11" t="s">
         <v>49</v>
       </c>
@@ -23404,7 +23404,7 @@
         <v>-9.7400000000000004E-4</v>
       </c>
     </row>
-    <row r="113" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="11" t="s">
         <v>47</v>
       </c>
@@ -23523,7 +23523,7 @@
         <v>4.7860000000000003E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="11" t="s">
         <v>45</v>
       </c>
@@ -23642,7 +23642,7 @@
         <v>6.5649999999999997E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="11" t="s">
         <v>43</v>
       </c>
@@ -23761,7 +23761,7 @@
         <v>8.744E-3</v>
       </c>
     </row>
-    <row r="116" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="11" t="s">
         <v>41</v>
       </c>
@@ -23880,8 +23880,8 @@
         <v>4.3969999999999999E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:39" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="118" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="35" t="s">
         <v>39</v>
       </c>
@@ -23923,107 +23923,107 @@
       <c r="AL118" s="35"/>
       <c r="AM118" s="35"/>
     </row>
-    <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="122" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B122" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="123" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B124" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="125" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B125" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B128" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B129" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="131" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B131" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="132" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B132" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="133" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="135" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B135" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="136" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B136" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B137" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B138" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B139" s="7" t="s">
         <v>18</v>
       </c>
@@ -24043,21 +24043,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>182</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2015</v>
       </c>
@@ -24167,7 +24167,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>345</v>
       </c>
@@ -24316,7 +24316,7 @@
         <v>2.0387429639167166E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>183</v>
       </c>
@@ -24325,19 +24325,19 @@
         <v>2.1866115765726366E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
         <v>184</v>
       </c>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B12" s="27" t="s">
         <v>344</v>
       </c>
@@ -24345,7 +24345,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>340</v>
       </c>
@@ -24353,7 +24353,7 @@
         <v>0.997</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>341</v>
       </c>
@@ -24361,7 +24361,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>342</v>
       </c>
@@ -24369,12 +24369,12 @@
         <v>0.96599999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>2015</v>
       </c>
@@ -24484,7 +24484,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>340</v>
       </c>
@@ -24629,7 +24629,7 @@
         <v>106.80688818099999</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>341</v>
       </c>
@@ -24774,7 +24774,7 @@
         <v>40.991097584999999</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>342</v>
       </c>
@@ -24919,12 +24919,12 @@
         <v>4.4407329119999996</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>2015</v>
       </c>
@@ -25034,7 +25034,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>340</v>
       </c>
@@ -25179,7 +25179,7 @@
         <v>1.1215938190000116</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>341</v>
       </c>
@@ -25324,7 +25324,7 @@
         <v>0.52974641499999819</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>342</v>
       </c>
@@ -25469,12 +25469,12 @@
         <v>0.12269708800000068</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>2015</v>
       </c>
@@ -25584,7 +25584,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>340</v>
       </c>
@@ -25729,7 +25729,7 @@
         <v>1.0501137502473678E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>341</v>
       </c>
@@ -25874,7 +25874,7 @@
         <v>1.2923450363862663E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>342</v>
       </c>
@@ -26019,15 +26019,15 @@
         <v>2.7629918401181404E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.35">
       <c r="C34" s="25"/>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>340</v>
       </c>
@@ -26036,7 +26036,7 @@
         <v>1.143000484613816E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>341</v>
       </c>
@@ -26045,7 +26045,7 @@
         <v>1.5514513735396921E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>342</v>
       </c>
@@ -26054,12 +26054,12 @@
         <v>2.7312273593190856E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>352</v>
       </c>
@@ -26068,34 +26068,34 @@
         <v>1.3254110935573082E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A44" s="30" t="s">
         <v>356</v>
       </c>
       <c r="B44" s="31"/>
       <c r="C44" s="31"/>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>361</v>
       </c>
@@ -26104,7 +26104,7 @@
         <v>0.97813388423427361</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>362</v>
       </c>
@@ -26113,12 +26113,12 @@
         <v>0.98674588906442695</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -26127,7 +26127,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -26136,7 +26136,7 @@
         <v>6.3157894736842107E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -26145,7 +26145,7 @@
         <v>0.1095</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -26154,7 +26154,7 @@
         <v>7.3891625615763554E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -26163,12 +26163,12 @@
         <v>6.4935064935064929E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>361</v>
       </c>
@@ -26176,7 +26176,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -26189,7 +26189,7 @@
         <v>6.5188105096858712E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -26202,7 +26202,7 @@
         <v>7.5574903929115839E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -26215,7 +26215,7 @@
         <v>0.12130278578812782</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -26228,7 +26228,7 @@
         <v>8.6166368748215469E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -26253,15 +26253,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.73046875" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" customWidth="1"/>
-    <col min="3" max="3" width="18.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.86328125" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="27" t="s">
         <v>353</v>
       </c>
@@ -26272,7 +26272,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -26289,7 +26289,7 @@
         <v>7.3346846514898659E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -26306,7 +26306,7 @@
         <v>8.3642992664733129E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -26320,7 +26320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -26337,7 +26337,7 @@
         <v>0.12897177608937932</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -26354,7 +26354,7 @@
         <v>9.4142018541657921E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -26371,7 +26371,7 @@
         <v>8.5381303053666202E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D8" s="4"/>
     </row>
   </sheetData>
@@ -26386,19 +26386,19 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.73046875" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" customWidth="1"/>
-    <col min="3" max="3" width="18.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.86328125" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
         <v>381</v>
       </c>
@@ -26412,7 +26412,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -26426,7 +26426,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -26440,7 +26440,7 @@
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -26454,7 +26454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -26468,21 +26468,21 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>7.2099999999999997E-2</v>
+        <v>0.08</v>
       </c>
       <c r="C6">
-        <v>7.2300000000000003E-2</v>
+        <v>0.08</v>
       </c>
       <c r="D6">
         <v>7.22E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -26496,7 +26496,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D8" s="4"/>
     </row>
   </sheetData>

</xml_diff>